<commit_message>
Adds plot legends and flattened network clusters draw method
</commit_message>
<xml_diff>
--- a/results/aucs/degree_centrality/aucs_degree_centrality_results.xlsx
+++ b/results/aucs/degree_centrality/aucs_degree_centrality_results.xlsx
@@ -685,7 +685,7 @@
         <v>1.95</v>
       </c>
       <c r="H3">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -711,7 +711,7 @@
         <v>0</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -737,7 +737,7 @@
         <v>1.69</v>
       </c>
       <c r="H5">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -763,7 +763,7 @@
         <v>1.82</v>
       </c>
       <c r="H6">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -789,7 +789,7 @@
         <v>1.69</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -815,7 +815,7 @@
         <v>2.16</v>
       </c>
       <c r="H8">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -841,7 +841,7 @@
         <v>1.5</v>
       </c>
       <c r="H9">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -867,7 +867,7 @@
         <v>1.85</v>
       </c>
       <c r="H10">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -945,7 +945,7 @@
         <v>1.6</v>
       </c>
       <c r="H13">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -971,7 +971,7 @@
         <v>1.23</v>
       </c>
       <c r="H14">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -997,7 +997,7 @@
         <v>1.72</v>
       </c>
       <c r="H15">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -1049,7 +1049,7 @@
         <v>1</v>
       </c>
       <c r="H17">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -1075,7 +1075,7 @@
         <v>1.79</v>
       </c>
       <c r="H18">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -1179,7 +1179,7 @@
         <v>1.02</v>
       </c>
       <c r="H22">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -1205,7 +1205,7 @@
         <v>1.6</v>
       </c>
       <c r="H23">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1231,7 +1231,7 @@
         <v>1.56</v>
       </c>
       <c r="H24">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1257,7 +1257,7 @@
         <v>2.05</v>
       </c>
       <c r="H25">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1309,7 +1309,7 @@
         <v>1.7</v>
       </c>
       <c r="H27">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1335,7 +1335,7 @@
         <v>1.42</v>
       </c>
       <c r="H28">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -1361,7 +1361,7 @@
         <v>1.52</v>
       </c>
       <c r="H29">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1413,7 +1413,7 @@
         <v>2.04</v>
       </c>
       <c r="H31">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1439,7 +1439,7 @@
         <v>1.65</v>
       </c>
       <c r="H32">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -1465,7 +1465,7 @@
         <v>1.68</v>
       </c>
       <c r="H33">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -1517,7 +1517,7 @@
         <v>1.1</v>
       </c>
       <c r="H35">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -1569,7 +1569,7 @@
         <v>1.44</v>
       </c>
       <c r="H37">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -1595,7 +1595,7 @@
         <v>1.74</v>
       </c>
       <c r="H38">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -1621,7 +1621,7 @@
         <v>1.73</v>
       </c>
       <c r="H39">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -1647,7 +1647,7 @@
         <v>1.08</v>
       </c>
       <c r="H40">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -1673,7 +1673,7 @@
         <v>1.57</v>
       </c>
       <c r="H41">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -1699,7 +1699,7 @@
         <v>1.44</v>
       </c>
       <c r="H42">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -1725,7 +1725,7 @@
         <v>1.97</v>
       </c>
       <c r="H43">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -1751,7 +1751,7 @@
         <v>1.78</v>
       </c>
       <c r="H44">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -1777,7 +1777,7 @@
         <v>1.67</v>
       </c>
       <c r="H45">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -1803,7 +1803,7 @@
         <v>1.19</v>
       </c>
       <c r="H46">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -1829,7 +1829,7 @@
         <v>0.95</v>
       </c>
       <c r="H47">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -1855,7 +1855,7 @@
         <v>1.91</v>
       </c>
       <c r="H48">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -1907,7 +1907,7 @@
         <v>1.54</v>
       </c>
       <c r="H50">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -1933,7 +1933,7 @@
         <v>1.76</v>
       </c>
       <c r="H51">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -1985,7 +1985,7 @@
         <v>1.53</v>
       </c>
       <c r="H53">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="54" spans="1:8">
@@ -2037,7 +2037,7 @@
         <v>2.07</v>
       </c>
       <c r="H55">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:8">
@@ -2063,7 +2063,7 @@
         <v>1.9</v>
       </c>
       <c r="H56">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:8">
@@ -2115,7 +2115,7 @@
         <v>1.55</v>
       </c>
       <c r="H58">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="59" spans="1:8">
@@ -2141,7 +2141,7 @@
         <v>1.88</v>
       </c>
       <c r="H59">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:8">
@@ -2167,7 +2167,7 @@
         <v>0.78</v>
       </c>
       <c r="H60">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="61" spans="1:8">
@@ -2193,7 +2193,7 @@
         <v>1.29</v>
       </c>
       <c r="H61">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="62" spans="1:8">
@@ -2219,7 +2219,7 @@
         <v>1.73</v>
       </c>
       <c r="H62">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="63" spans="1:8">
@@ -2245,7 +2245,7 @@
         <v>1.47</v>
       </c>
       <c r="H63">
-        <v>1.02</v>
+        <v>1.05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adds function test modules, game theoretic centrality modules, refactors algo modules and helper modules
</commit_message>
<xml_diff>
--- a/results/aucs/degree_centrality/aucs_degree_centrality_results.xlsx
+++ b/results/aucs/degree_centrality/aucs_degree_centrality_results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="70">
   <si>
     <t>coauthor</t>
   </si>
@@ -221,6 +221,9 @@
   </si>
   <si>
     <t>mean</t>
+  </si>
+  <si>
+    <t>-inf</t>
   </si>
 </sst>
 </file>
@@ -641,25 +644,25 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>1.43</v>
+        <v>2.12</v>
       </c>
       <c r="C2">
-        <v>21.67</v>
+        <v>30.26</v>
       </c>
       <c r="D2">
-        <v>12.14</v>
+        <v>12.53</v>
       </c>
       <c r="E2">
-        <v>18.1</v>
+        <v>13.01</v>
       </c>
       <c r="F2">
-        <v>46.67</v>
+        <v>42.07</v>
       </c>
       <c r="G2">
-        <v>1.89</v>
+        <v>1.92</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -667,22 +670,22 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>1.54</v>
+        <v>2.48</v>
       </c>
       <c r="C3">
-        <v>24.62</v>
+        <v>31.93</v>
       </c>
       <c r="D3">
-        <v>28.46</v>
+        <v>29.82</v>
       </c>
       <c r="E3">
-        <v>9.23</v>
+        <v>4.2</v>
       </c>
       <c r="F3">
-        <v>36.15</v>
+        <v>31.58</v>
       </c>
       <c r="G3">
-        <v>1.95</v>
+        <v>1.9</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -719,22 +722,22 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <v>1.79</v>
+        <v>2.55</v>
       </c>
       <c r="C5">
-        <v>46.43</v>
+        <v>57.18</v>
       </c>
       <c r="D5">
-        <v>4.17</v>
+        <v>2.4</v>
       </c>
       <c r="E5">
-        <v>36.31</v>
+        <v>31.65</v>
       </c>
       <c r="F5">
-        <v>11.31</v>
+        <v>6.22</v>
       </c>
       <c r="G5">
-        <v>1.69</v>
+        <v>1.5</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -748,19 +751,19 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <v>34.76</v>
+        <v>47.71</v>
       </c>
       <c r="D6">
-        <v>17.59</v>
+        <v>17</v>
       </c>
       <c r="E6">
-        <v>9.41</v>
+        <v>3.52</v>
       </c>
       <c r="F6">
-        <v>38.24</v>
+        <v>31.77</v>
       </c>
       <c r="G6">
-        <v>1.82</v>
+        <v>1.64</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -774,22 +777,22 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <v>19.43</v>
+        <v>30.89</v>
       </c>
       <c r="D7">
-        <v>11.77</v>
+        <v>11.88</v>
       </c>
       <c r="E7">
-        <v>55.18</v>
+        <v>49.48</v>
       </c>
       <c r="F7">
-        <v>13.62</v>
+        <v>7.75</v>
       </c>
       <c r="G7">
-        <v>1.69</v>
+        <v>1.68</v>
       </c>
       <c r="H7">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -797,22 +800,22 @@
         <v>13</v>
       </c>
       <c r="B8">
-        <v>9.82</v>
+        <v>15.08</v>
       </c>
       <c r="C8">
-        <v>23.86</v>
+        <v>32.51</v>
       </c>
       <c r="D8">
-        <v>14.21</v>
+        <v>13.23</v>
       </c>
       <c r="E8">
-        <v>15.09</v>
+        <v>8.44</v>
       </c>
       <c r="F8">
-        <v>37.02</v>
+        <v>30.75</v>
       </c>
       <c r="G8">
-        <v>2.16</v>
+        <v>2.15</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -826,19 +829,19 @@
         <v>0</v>
       </c>
       <c r="C9">
-        <v>42.62</v>
+        <v>52.7</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
       <c r="E9">
-        <v>39.34</v>
+        <v>33.82</v>
       </c>
       <c r="F9">
-        <v>18.03</v>
+        <v>13.48</v>
       </c>
       <c r="G9">
-        <v>1.5</v>
+        <v>1.41</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -852,19 +855,19 @@
         <v>0</v>
       </c>
       <c r="C10">
-        <v>38.72</v>
+        <v>53.74</v>
       </c>
       <c r="D10">
-        <v>15.11</v>
+        <v>15.12</v>
       </c>
       <c r="E10">
-        <v>33.13</v>
+        <v>24.99</v>
       </c>
       <c r="F10">
-        <v>13.04</v>
+        <v>6.15</v>
       </c>
       <c r="G10">
-        <v>1.85</v>
+        <v>1.64</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -875,22 +878,22 @@
         <v>16</v>
       </c>
       <c r="B11">
-        <v>3.62</v>
+        <v>10.27</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="D11">
-        <v>3.62</v>
+        <v>3.63</v>
       </c>
       <c r="E11">
-        <v>33.48</v>
+        <v>30.34</v>
       </c>
       <c r="F11">
-        <v>59.28</v>
+        <v>55.76</v>
       </c>
       <c r="G11">
-        <v>1.32</v>
+        <v>1.5</v>
       </c>
       <c r="H11">
         <v>1</v>
@@ -904,19 +907,19 @@
         <v>0</v>
       </c>
       <c r="C12">
-        <v>19.6</v>
+        <v>32.62</v>
       </c>
       <c r="D12">
         <v>0</v>
       </c>
       <c r="E12">
-        <v>7.35</v>
+        <v>2.13</v>
       </c>
       <c r="F12">
-        <v>73.05</v>
+        <v>65.25</v>
       </c>
       <c r="G12">
-        <v>1.07</v>
+        <v>1.05</v>
       </c>
       <c r="H12">
         <v>1</v>
@@ -930,19 +933,19 @@
         <v>0</v>
       </c>
       <c r="C13">
-        <v>58.81</v>
+        <v>76.22</v>
       </c>
       <c r="D13">
-        <v>10.75</v>
+        <v>8.460000000000001</v>
       </c>
       <c r="E13">
-        <v>10.75</v>
+        <v>3.42</v>
       </c>
       <c r="F13">
-        <v>19.7</v>
+        <v>11.9</v>
       </c>
       <c r="G13">
-        <v>1.6</v>
+        <v>1.13</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -959,13 +962,13 @@
         <v>0</v>
       </c>
       <c r="D14">
-        <v>25.87</v>
+        <v>32.95</v>
       </c>
       <c r="E14">
-        <v>64.68000000000001</v>
+        <v>60.44</v>
       </c>
       <c r="F14">
-        <v>9.449999999999999</v>
+        <v>6.6</v>
       </c>
       <c r="G14">
         <v>1.23</v>
@@ -979,22 +982,22 @@
         <v>20</v>
       </c>
       <c r="B15">
-        <v>6.87</v>
+        <v>12.65</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
       <c r="D15">
-        <v>14.5</v>
+        <v>14.14</v>
       </c>
       <c r="E15">
-        <v>35.88</v>
+        <v>32.97</v>
       </c>
       <c r="F15">
-        <v>42.75</v>
+        <v>40.23</v>
       </c>
       <c r="G15">
-        <v>1.72</v>
+        <v>1.83</v>
       </c>
       <c r="H15">
         <v>2</v>
@@ -1005,25 +1008,25 @@
         <v>21</v>
       </c>
       <c r="B16">
-        <v>7.87</v>
+        <v>14.88</v>
       </c>
       <c r="C16">
-        <v>29.66</v>
+        <v>42.32</v>
       </c>
       <c r="D16">
         <v>0</v>
       </c>
       <c r="E16">
-        <v>15.49</v>
+        <v>5.66</v>
       </c>
       <c r="F16">
-        <v>46.98</v>
+        <v>37.14</v>
       </c>
       <c r="G16">
-        <v>1.74</v>
+        <v>1.7</v>
       </c>
       <c r="H16">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -1031,22 +1034,22 @@
         <v>22</v>
       </c>
       <c r="B17">
-        <v>1.65</v>
+        <v>4.12</v>
       </c>
       <c r="C17">
-        <v>9.5</v>
+        <v>12.8</v>
       </c>
       <c r="D17">
         <v>0</v>
       </c>
       <c r="E17">
-        <v>79.75</v>
+        <v>76.73999999999999</v>
       </c>
       <c r="F17">
-        <v>9.09</v>
+        <v>6.34</v>
       </c>
       <c r="G17">
-        <v>1</v>
+        <v>1.11</v>
       </c>
       <c r="H17">
         <v>2</v>
@@ -1057,22 +1060,22 @@
         <v>23</v>
       </c>
       <c r="B18">
-        <v>5.25</v>
+        <v>11.25</v>
       </c>
       <c r="C18">
         <v>0</v>
       </c>
       <c r="D18">
-        <v>27.16</v>
+        <v>32</v>
       </c>
       <c r="E18">
-        <v>31.17</v>
+        <v>25.55</v>
       </c>
       <c r="F18">
-        <v>36.42</v>
+        <v>31.2</v>
       </c>
       <c r="G18">
-        <v>1.79</v>
+        <v>1.91</v>
       </c>
       <c r="H18">
         <v>2</v>
@@ -1092,13 +1095,13 @@
         <v>0</v>
       </c>
       <c r="E19">
-        <v>8.33</v>
+        <v>7.63</v>
       </c>
       <c r="F19">
-        <v>91.67</v>
+        <v>92.37</v>
       </c>
       <c r="G19">
-        <v>0.41</v>
+        <v>0.39</v>
       </c>
       <c r="H19">
         <v>1</v>
@@ -1115,19 +1118,19 @@
         <v>0</v>
       </c>
       <c r="D20">
-        <v>14.15</v>
+        <v>21.74</v>
       </c>
       <c r="E20">
-        <v>36.79</v>
+        <v>34.05</v>
       </c>
       <c r="F20">
-        <v>49.06</v>
+        <v>44.22</v>
       </c>
       <c r="G20">
-        <v>1.43</v>
+        <v>1.53</v>
       </c>
       <c r="H20">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -1167,16 +1170,16 @@
         <v>0</v>
       </c>
       <c r="D22">
-        <v>6.52</v>
+        <v>10.87</v>
       </c>
       <c r="E22">
-        <v>75</v>
+        <v>69.98999999999999</v>
       </c>
       <c r="F22">
-        <v>18.48</v>
+        <v>19.14</v>
       </c>
       <c r="G22">
-        <v>1.02</v>
+        <v>1.16</v>
       </c>
       <c r="H22">
         <v>2</v>
@@ -1187,22 +1190,22 @@
         <v>28</v>
       </c>
       <c r="B23">
-        <v>2.38</v>
+        <v>2.27</v>
       </c>
       <c r="C23">
-        <v>63.1</v>
+        <v>79.90000000000001</v>
       </c>
       <c r="D23">
-        <v>16.67</v>
+        <v>14.67</v>
       </c>
       <c r="E23">
-        <v>9.52</v>
+        <v>2.19</v>
       </c>
       <c r="F23">
-        <v>8.33</v>
+        <v>0.98</v>
       </c>
       <c r="G23">
-        <v>1.6</v>
+        <v>0.97</v>
       </c>
       <c r="H23">
         <v>0</v>
@@ -1219,16 +1222,16 @@
         <v>0</v>
       </c>
       <c r="D24">
-        <v>29.76</v>
+        <v>35.58</v>
       </c>
       <c r="E24">
-        <v>27.38</v>
+        <v>25.86</v>
       </c>
       <c r="F24">
-        <v>42.86</v>
+        <v>38.57</v>
       </c>
       <c r="G24">
-        <v>1.56</v>
+        <v>1.57</v>
       </c>
       <c r="H24">
         <v>2</v>
@@ -1239,22 +1242,22 @@
         <v>30</v>
       </c>
       <c r="B25">
-        <v>4.86</v>
+        <v>7.87</v>
       </c>
       <c r="C25">
-        <v>34.03</v>
+        <v>47.07</v>
       </c>
       <c r="D25">
-        <v>13.19</v>
+        <v>11.55</v>
       </c>
       <c r="E25">
-        <v>34.03</v>
+        <v>27</v>
       </c>
       <c r="F25">
-        <v>13.89</v>
+        <v>6.52</v>
       </c>
       <c r="G25">
-        <v>2.05</v>
+        <v>1.93</v>
       </c>
       <c r="H25">
         <v>0</v>
@@ -1271,16 +1274,16 @@
         <v>0</v>
       </c>
       <c r="D26">
-        <v>10.23</v>
+        <v>16.3</v>
       </c>
       <c r="E26">
-        <v>22.73</v>
+        <v>22.78</v>
       </c>
       <c r="F26">
-        <v>67.05</v>
+        <v>60.92</v>
       </c>
       <c r="G26">
-        <v>1.21</v>
+        <v>1.35</v>
       </c>
       <c r="H26">
         <v>1</v>
@@ -1294,19 +1297,19 @@
         <v>0</v>
       </c>
       <c r="C27">
-        <v>29.02</v>
+        <v>41.6</v>
       </c>
       <c r="D27">
-        <v>6.12</v>
+        <v>4.26</v>
       </c>
       <c r="E27">
-        <v>48.07</v>
+        <v>42.96</v>
       </c>
       <c r="F27">
-        <v>16.78</v>
+        <v>11.18</v>
       </c>
       <c r="G27">
-        <v>1.7</v>
+        <v>1.6</v>
       </c>
       <c r="H27">
         <v>0</v>
@@ -1317,22 +1320,22 @@
         <v>33</v>
       </c>
       <c r="B28">
-        <v>4.46</v>
+        <v>10.23</v>
       </c>
       <c r="C28">
         <v>0</v>
       </c>
       <c r="D28">
-        <v>4.46</v>
+        <v>4.54</v>
       </c>
       <c r="E28">
-        <v>53.02</v>
+        <v>49.88</v>
       </c>
       <c r="F28">
-        <v>38.06</v>
+        <v>35.35</v>
       </c>
       <c r="G28">
-        <v>1.42</v>
+        <v>1.57</v>
       </c>
       <c r="H28">
         <v>2</v>
@@ -1349,16 +1352,16 @@
         <v>0</v>
       </c>
       <c r="D29">
-        <v>25.86</v>
+        <v>36.23</v>
       </c>
       <c r="E29">
-        <v>25.86</v>
+        <v>23.41</v>
       </c>
       <c r="F29">
-        <v>48.28</v>
+        <v>40.36</v>
       </c>
       <c r="G29">
-        <v>1.52</v>
+        <v>1.55</v>
       </c>
       <c r="H29">
         <v>2</v>
@@ -1369,22 +1372,22 @@
         <v>35</v>
       </c>
       <c r="B30">
-        <v>1.79</v>
+        <v>4.21</v>
       </c>
       <c r="C30">
         <v>0</v>
       </c>
       <c r="D30">
-        <v>2.85</v>
+        <v>2.87</v>
       </c>
       <c r="E30">
-        <v>19.2</v>
+        <v>18.05</v>
       </c>
       <c r="F30">
-        <v>76.16</v>
+        <v>74.87</v>
       </c>
       <c r="G30">
-        <v>1.01</v>
+        <v>1.1</v>
       </c>
       <c r="H30">
         <v>1</v>
@@ -1395,22 +1398,22 @@
         <v>36</v>
       </c>
       <c r="B31">
-        <v>2.22</v>
+        <v>3.84</v>
       </c>
       <c r="C31">
-        <v>33.7</v>
+        <v>44.92</v>
       </c>
       <c r="D31">
-        <v>13.33</v>
+        <v>11.69</v>
       </c>
       <c r="E31">
-        <v>28.15</v>
+        <v>22.6</v>
       </c>
       <c r="F31">
-        <v>22.59</v>
+        <v>16.95</v>
       </c>
       <c r="G31">
-        <v>2.04</v>
+        <v>1.98</v>
       </c>
       <c r="H31">
         <v>0</v>
@@ -1424,19 +1427,19 @@
         <v>0</v>
       </c>
       <c r="C32">
-        <v>44.39</v>
+        <v>59.67</v>
       </c>
       <c r="D32">
-        <v>5.61</v>
+        <v>3.57</v>
       </c>
       <c r="E32">
-        <v>37.79</v>
+        <v>31.48</v>
       </c>
       <c r="F32">
-        <v>12.21</v>
+        <v>5.28</v>
       </c>
       <c r="G32">
-        <v>1.65</v>
+        <v>1.37</v>
       </c>
       <c r="H32">
         <v>0</v>
@@ -1447,22 +1450,22 @@
         <v>38</v>
       </c>
       <c r="B33">
-        <v>1.18</v>
+        <v>1.04</v>
       </c>
       <c r="C33">
-        <v>44.8</v>
+        <v>58.56</v>
       </c>
       <c r="D33">
-        <v>2.65</v>
+        <v>0.02</v>
       </c>
       <c r="E33">
-        <v>15.39</v>
+        <v>9.720000000000001</v>
       </c>
       <c r="F33">
-        <v>35.98</v>
+        <v>30.66</v>
       </c>
       <c r="G33">
-        <v>1.68</v>
+        <v>1.37</v>
       </c>
       <c r="H33">
         <v>0</v>
@@ -1482,13 +1485,13 @@
         <v>0</v>
       </c>
       <c r="E34">
-        <v>30.91</v>
+        <v>34.75</v>
       </c>
       <c r="F34">
-        <v>69.09</v>
+        <v>65.25</v>
       </c>
       <c r="G34">
-        <v>0.89</v>
+        <v>0.93</v>
       </c>
       <c r="H34">
         <v>1</v>
@@ -1505,16 +1508,16 @@
         <v>0</v>
       </c>
       <c r="D35">
-        <v>25.49</v>
+        <v>27.68</v>
       </c>
       <c r="E35">
-        <v>69.12</v>
+        <v>67.94</v>
       </c>
       <c r="F35">
-        <v>5.39</v>
+        <v>4.38</v>
       </c>
       <c r="G35">
-        <v>1.1</v>
+        <v>1.09</v>
       </c>
       <c r="H35">
         <v>2</v>
@@ -1528,22 +1531,22 @@
         <v>0</v>
       </c>
       <c r="C36">
-        <v>29.65</v>
+        <v>40.67</v>
       </c>
       <c r="D36">
-        <v>0.85</v>
+        <v>-1.67</v>
       </c>
       <c r="E36">
-        <v>24.77</v>
+        <v>20.72</v>
       </c>
       <c r="F36">
-        <v>44.73</v>
-      </c>
-      <c r="G36">
-        <v>1.6</v>
+        <v>40.27</v>
+      </c>
+      <c r="G36" t="s">
+        <v>69</v>
       </c>
       <c r="H36">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -1551,22 +1554,22 @@
         <v>42</v>
       </c>
       <c r="B37">
-        <v>4.49</v>
+        <v>12.15</v>
       </c>
       <c r="C37">
         <v>0</v>
       </c>
       <c r="D37">
-        <v>10.86</v>
+        <v>12.88</v>
       </c>
       <c r="E37">
-        <v>63.67</v>
+        <v>57.82</v>
       </c>
       <c r="F37">
-        <v>20.97</v>
+        <v>17.15</v>
       </c>
       <c r="G37">
-        <v>1.44</v>
+        <v>1.64</v>
       </c>
       <c r="H37">
         <v>2</v>
@@ -1580,19 +1583,19 @@
         <v>0</v>
       </c>
       <c r="C38">
-        <v>16.21</v>
+        <v>25.83</v>
       </c>
       <c r="D38">
-        <v>14.36</v>
+        <v>15.72</v>
       </c>
       <c r="E38">
-        <v>53.22</v>
+        <v>47.02</v>
       </c>
       <c r="F38">
-        <v>16.21</v>
+        <v>11.43</v>
       </c>
       <c r="G38">
-        <v>1.74</v>
+        <v>1.79</v>
       </c>
       <c r="H38">
         <v>2</v>
@@ -1603,22 +1606,22 @@
         <v>44</v>
       </c>
       <c r="B39">
-        <v>4.76</v>
+        <v>7.1</v>
       </c>
       <c r="C39">
-        <v>55.95</v>
+        <v>72.41</v>
       </c>
       <c r="D39">
-        <v>3.57</v>
+        <v>-0.5600000000000001</v>
       </c>
       <c r="E39">
-        <v>20.24</v>
+        <v>12.95</v>
       </c>
       <c r="F39">
-        <v>15.48</v>
-      </c>
-      <c r="G39">
-        <v>1.73</v>
+        <v>8.109999999999999</v>
+      </c>
+      <c r="G39" t="s">
+        <v>69</v>
       </c>
       <c r="H39">
         <v>0</v>
@@ -1629,7 +1632,7 @@
         <v>45</v>
       </c>
       <c r="B40">
-        <v>5.5</v>
+        <v>12.54</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -1638,13 +1641,13 @@
         <v>0</v>
       </c>
       <c r="E40">
-        <v>70.5</v>
+        <v>65.98</v>
       </c>
       <c r="F40">
-        <v>24</v>
+        <v>21.49</v>
       </c>
       <c r="G40">
-        <v>1.08</v>
+        <v>1.25</v>
       </c>
       <c r="H40">
         <v>2</v>
@@ -1658,19 +1661,19 @@
         <v>0</v>
       </c>
       <c r="C41">
-        <v>13.46</v>
+        <v>21.82</v>
       </c>
       <c r="D41">
-        <v>5.2</v>
+        <v>4.74</v>
       </c>
       <c r="E41">
-        <v>56.57</v>
+        <v>52.26</v>
       </c>
       <c r="F41">
-        <v>24.77</v>
+        <v>21.18</v>
       </c>
       <c r="G41">
-        <v>1.57</v>
+        <v>1.65</v>
       </c>
       <c r="H41">
         <v>2</v>
@@ -1681,22 +1684,22 @@
         <v>47</v>
       </c>
       <c r="B42">
-        <v>20.97</v>
+        <v>44.72</v>
       </c>
       <c r="C42">
         <v>0</v>
       </c>
       <c r="D42">
-        <v>4.49</v>
+        <v>0.02</v>
       </c>
       <c r="E42">
-        <v>63.67</v>
+        <v>53.05</v>
       </c>
       <c r="F42">
-        <v>10.86</v>
+        <v>2.21</v>
       </c>
       <c r="G42">
-        <v>1.44</v>
+        <v>1.13</v>
       </c>
       <c r="H42">
         <v>2</v>
@@ -1710,19 +1713,19 @@
         <v>0</v>
       </c>
       <c r="C43">
-        <v>29.95</v>
+        <v>42.22</v>
       </c>
       <c r="D43">
-        <v>17.97</v>
+        <v>18.6</v>
       </c>
       <c r="E43">
-        <v>23.48</v>
+        <v>17.36</v>
       </c>
       <c r="F43">
-        <v>28.6</v>
+        <v>21.82</v>
       </c>
       <c r="G43">
-        <v>1.97</v>
+        <v>1.89</v>
       </c>
       <c r="H43">
         <v>0</v>
@@ -1736,19 +1739,19 @@
         <v>0</v>
       </c>
       <c r="C44">
-        <v>32.09</v>
+        <v>44.62</v>
       </c>
       <c r="D44">
-        <v>16.15</v>
+        <v>16.92</v>
       </c>
       <c r="E44">
-        <v>43.27</v>
+        <v>36.18</v>
       </c>
       <c r="F44">
-        <v>8.49</v>
+        <v>2.28</v>
       </c>
       <c r="G44">
-        <v>1.78</v>
+        <v>1.61</v>
       </c>
       <c r="H44">
         <v>0</v>
@@ -1762,19 +1765,19 @@
         <v>0</v>
       </c>
       <c r="C45">
-        <v>27.54</v>
+        <v>38.86</v>
       </c>
       <c r="D45">
-        <v>5.39</v>
+        <v>3.78</v>
       </c>
       <c r="E45">
-        <v>50.3</v>
+        <v>45.62</v>
       </c>
       <c r="F45">
-        <v>16.77</v>
+        <v>11.73</v>
       </c>
       <c r="G45">
-        <v>1.67</v>
+        <v>1.59</v>
       </c>
       <c r="H45">
         <v>0</v>
@@ -1791,16 +1794,16 @@
         <v>0</v>
       </c>
       <c r="D46">
-        <v>4.51</v>
+        <v>7.91</v>
       </c>
       <c r="E46">
-        <v>57.52</v>
+        <v>55.29</v>
       </c>
       <c r="F46">
-        <v>37.97</v>
+        <v>36.8</v>
       </c>
       <c r="G46">
-        <v>1.19</v>
+        <v>1.29</v>
       </c>
       <c r="H46">
         <v>2</v>
@@ -1820,13 +1823,13 @@
         <v>0</v>
       </c>
       <c r="E47">
-        <v>62.96</v>
+        <v>58.47</v>
       </c>
       <c r="F47">
-        <v>37.04</v>
+        <v>41.53</v>
       </c>
       <c r="G47">
-        <v>0.95</v>
+        <v>0.98</v>
       </c>
       <c r="H47">
         <v>2</v>
@@ -1840,19 +1843,19 @@
         <v>0</v>
       </c>
       <c r="C48">
-        <v>25.31</v>
+        <v>34.97</v>
       </c>
       <c r="D48">
-        <v>34.36</v>
+        <v>37.17</v>
       </c>
       <c r="E48">
-        <v>28.81</v>
+        <v>22.4</v>
       </c>
       <c r="F48">
-        <v>11.52</v>
+        <v>5.46</v>
       </c>
       <c r="G48">
-        <v>1.91</v>
+        <v>1.77</v>
       </c>
       <c r="H48">
         <v>0</v>
@@ -1866,22 +1869,22 @@
         <v>0</v>
       </c>
       <c r="C49">
-        <v>28.73</v>
+        <v>42.56</v>
       </c>
       <c r="D49">
-        <v>2.34</v>
+        <v>-0.37</v>
       </c>
       <c r="E49">
-        <v>20.1</v>
+        <v>14.91</v>
       </c>
       <c r="F49">
-        <v>48.83</v>
-      </c>
-      <c r="G49">
-        <v>1.61</v>
+        <v>42.91</v>
+      </c>
+      <c r="G49" t="s">
+        <v>69</v>
       </c>
       <c r="H49">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -1889,22 +1892,22 @@
         <v>55</v>
       </c>
       <c r="B50">
-        <v>5.25</v>
+        <v>11.54</v>
       </c>
       <c r="C50">
         <v>0</v>
       </c>
       <c r="D50">
-        <v>10.49</v>
+        <v>12.14</v>
       </c>
       <c r="E50">
-        <v>57.1</v>
+        <v>52.28</v>
       </c>
       <c r="F50">
-        <v>27.16</v>
+        <v>24.03</v>
       </c>
       <c r="G50">
-        <v>1.54</v>
+        <v>1.71</v>
       </c>
       <c r="H50">
         <v>2</v>
@@ -1918,19 +1921,19 @@
         <v>0</v>
       </c>
       <c r="C51">
-        <v>36.45</v>
+        <v>49.8</v>
       </c>
       <c r="D51">
-        <v>7.22</v>
+        <v>5.67</v>
       </c>
       <c r="E51">
-        <v>39.74</v>
+        <v>33.82</v>
       </c>
       <c r="F51">
-        <v>16.58</v>
+        <v>10.71</v>
       </c>
       <c r="G51">
-        <v>1.76</v>
+        <v>1.61</v>
       </c>
       <c r="H51">
         <v>0</v>
@@ -1944,19 +1947,19 @@
         <v>0</v>
       </c>
       <c r="C52">
-        <v>24.52</v>
+        <v>38.97</v>
       </c>
       <c r="D52">
         <v>0</v>
       </c>
       <c r="E52">
-        <v>12.14</v>
+        <v>6.5</v>
       </c>
       <c r="F52">
-        <v>63.33</v>
+        <v>54.53</v>
       </c>
       <c r="G52">
-        <v>1.28</v>
+        <v>1.26</v>
       </c>
       <c r="H52">
         <v>1</v>
@@ -1967,22 +1970,22 @@
         <v>58</v>
       </c>
       <c r="B53">
-        <v>7.22</v>
+        <v>14.85</v>
       </c>
       <c r="C53">
         <v>0</v>
       </c>
       <c r="D53">
-        <v>15.37</v>
+        <v>17.27</v>
       </c>
       <c r="E53">
-        <v>62.04</v>
+        <v>56.82</v>
       </c>
       <c r="F53">
-        <v>15.37</v>
+        <v>11.06</v>
       </c>
       <c r="G53">
-        <v>1.53</v>
+        <v>1.66</v>
       </c>
       <c r="H53">
         <v>2</v>
@@ -1999,16 +2002,16 @@
         <v>0</v>
       </c>
       <c r="D54">
-        <v>41.88</v>
+        <v>48.57</v>
       </c>
       <c r="E54">
-        <v>25.62</v>
+        <v>22.54</v>
       </c>
       <c r="F54">
-        <v>32.5</v>
+        <v>28.89</v>
       </c>
       <c r="G54">
-        <v>1.56</v>
+        <v>1.51</v>
       </c>
       <c r="H54">
         <v>2</v>
@@ -2019,22 +2022,22 @@
         <v>60</v>
       </c>
       <c r="B55">
-        <v>3.89</v>
+        <v>5.81</v>
       </c>
       <c r="C55">
-        <v>33.89</v>
+        <v>46.85</v>
       </c>
       <c r="D55">
-        <v>17.22</v>
+        <v>16.73</v>
       </c>
       <c r="E55">
-        <v>30.56</v>
+        <v>23.5</v>
       </c>
       <c r="F55">
-        <v>14.44</v>
+        <v>7.12</v>
       </c>
       <c r="G55">
-        <v>2.07</v>
+        <v>1.94</v>
       </c>
       <c r="H55">
         <v>0</v>
@@ -2048,19 +2051,19 @@
         <v>0</v>
       </c>
       <c r="C56">
-        <v>36.7</v>
+        <v>51.63</v>
       </c>
       <c r="D56">
-        <v>13.3</v>
+        <v>12.05</v>
       </c>
       <c r="E56">
-        <v>30.28</v>
+        <v>23.46</v>
       </c>
       <c r="F56">
-        <v>19.72</v>
+        <v>12.86</v>
       </c>
       <c r="G56">
-        <v>1.9</v>
+        <v>1.73</v>
       </c>
       <c r="H56">
         <v>0</v>
@@ -2080,10 +2083,10 @@
         <v>0</v>
       </c>
       <c r="E57">
-        <v>33.33</v>
+        <v>33.05</v>
       </c>
       <c r="F57">
-        <v>66.67</v>
+        <v>66.95</v>
       </c>
       <c r="G57">
         <v>0.92</v>
@@ -2103,13 +2106,13 @@
         <v>0</v>
       </c>
       <c r="D58">
-        <v>28.35</v>
+        <v>35.7</v>
       </c>
       <c r="E58">
-        <v>44.21</v>
+        <v>41.23</v>
       </c>
       <c r="F58">
-        <v>27.44</v>
+        <v>23.07</v>
       </c>
       <c r="G58">
         <v>1.55</v>
@@ -2123,22 +2126,22 @@
         <v>64</v>
       </c>
       <c r="B59">
-        <v>3.18</v>
+        <v>5.25</v>
       </c>
       <c r="C59">
-        <v>42.58</v>
+        <v>55.04</v>
       </c>
       <c r="D59">
-        <v>34.24</v>
+        <v>35.28</v>
       </c>
       <c r="E59">
-        <v>9.24</v>
+        <v>1.44</v>
       </c>
       <c r="F59">
-        <v>10.76</v>
+        <v>2.99</v>
       </c>
       <c r="G59">
-        <v>1.88</v>
+        <v>1.47</v>
       </c>
       <c r="H59">
         <v>0</v>
@@ -2158,13 +2161,13 @@
         <v>0</v>
       </c>
       <c r="E60">
-        <v>76.92</v>
+        <v>75.42</v>
       </c>
       <c r="F60">
-        <v>23.08</v>
+        <v>24.58</v>
       </c>
       <c r="G60">
-        <v>0.78</v>
+        <v>0.8</v>
       </c>
       <c r="H60">
         <v>2</v>
@@ -2175,7 +2178,7 @@
         <v>66</v>
       </c>
       <c r="B61">
-        <v>6.81</v>
+        <v>10.04</v>
       </c>
       <c r="C61">
         <v>0</v>
@@ -2184,13 +2187,13 @@
         <v>0</v>
       </c>
       <c r="E61">
-        <v>46.6</v>
+        <v>44.98</v>
       </c>
       <c r="F61">
-        <v>46.6</v>
+        <v>44.98</v>
       </c>
       <c r="G61">
-        <v>1.29</v>
+        <v>1.37</v>
       </c>
       <c r="H61">
         <v>2</v>
@@ -2201,22 +2204,22 @@
         <v>67</v>
       </c>
       <c r="B62">
-        <v>8.06</v>
+        <v>15.93</v>
       </c>
       <c r="C62">
         <v>0</v>
       </c>
       <c r="D62">
-        <v>13</v>
+        <v>14.01</v>
       </c>
       <c r="E62">
-        <v>41.94</v>
+        <v>37.57</v>
       </c>
       <c r="F62">
-        <v>37</v>
+        <v>32.49</v>
       </c>
       <c r="G62">
-        <v>1.73</v>
+        <v>1.88</v>
       </c>
       <c r="H62">
         <v>2</v>
@@ -2227,25 +2230,25 @@
         <v>68</v>
       </c>
       <c r="B63">
-        <v>2.08</v>
+        <v>4.01</v>
       </c>
       <c r="C63">
-        <v>17.24</v>
+        <v>23.59</v>
       </c>
       <c r="D63">
-        <v>10.88</v>
+        <v>11.59</v>
       </c>
       <c r="E63">
-        <v>37.45</v>
+        <v>32.94</v>
       </c>
       <c r="F63">
-        <v>32.35</v>
-      </c>
-      <c r="G63">
-        <v>1.47</v>
+        <v>27.87</v>
+      </c>
+      <c r="G63" t="s">
+        <v>69</v>
       </c>
       <c r="H63">
-        <v>1.05</v>
+        <v>0.97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removes cluster from degree centrality
</commit_message>
<xml_diff>
--- a/results/aucs/degree_centrality/aucs_degree_centrality_results.xlsx
+++ b/results/aucs/degree_centrality/aucs_degree_centrality_results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
   <si>
     <t>coauthor</t>
   </si>
@@ -32,9 +32,6 @@
   </si>
   <si>
     <t>shannon_entropy</t>
-  </si>
-  <si>
-    <t>cluster_class</t>
   </si>
   <si>
     <t>U1</t>
@@ -607,13 +604,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H63"/>
+  <dimension ref="A1:G63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:7">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -632,13 +629,10 @@
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="1" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="B2">
         <v>1.43</v>
@@ -658,13 +652,10 @@
       <c r="G2">
         <v>1.89</v>
       </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3">
         <v>1.54</v>
@@ -684,13 +675,10 @@
       <c r="G3">
         <v>1.95</v>
       </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -710,13 +698,10 @@
       <c r="G4">
         <v>0</v>
       </c>
-      <c r="H4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5">
         <v>1.79</v>
@@ -736,13 +721,10 @@
       <c r="G5">
         <v>1.69</v>
       </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -762,13 +744,10 @@
       <c r="G6">
         <v>1.82</v>
       </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -788,13 +767,10 @@
       <c r="G7">
         <v>1.69</v>
       </c>
-      <c r="H7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8">
         <v>9.82</v>
@@ -814,13 +790,10 @@
       <c r="G8">
         <v>2.16</v>
       </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -840,13 +813,10 @@
       <c r="G9">
         <v>1.5</v>
       </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -866,13 +836,10 @@
       <c r="G10">
         <v>1.85</v>
       </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11">
         <v>3.62</v>
@@ -892,13 +859,10 @@
       <c r="G11">
         <v>1.32</v>
       </c>
-      <c r="H11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -918,13 +882,10 @@
       <c r="G12">
         <v>1.07</v>
       </c>
-      <c r="H12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -944,13 +905,10 @@
       <c r="G13">
         <v>1.6</v>
       </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -970,13 +928,10 @@
       <c r="G14">
         <v>1.23</v>
       </c>
-      <c r="H14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15">
         <v>6.87</v>
@@ -996,13 +951,10 @@
       <c r="G15">
         <v>1.72</v>
       </c>
-      <c r="H15">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B16">
         <v>7.87</v>
@@ -1022,13 +974,10 @@
       <c r="G16">
         <v>1.74</v>
       </c>
-      <c r="H16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B17">
         <v>1.65</v>
@@ -1048,13 +997,10 @@
       <c r="G17">
         <v>1</v>
       </c>
-      <c r="H17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B18">
         <v>5.25</v>
@@ -1074,13 +1020,10 @@
       <c r="G18">
         <v>1.79</v>
       </c>
-      <c r="H18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -1100,13 +1043,10 @@
       <c r="G19">
         <v>0.41</v>
       </c>
-      <c r="H19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -1126,13 +1066,10 @@
       <c r="G20">
         <v>1.43</v>
       </c>
-      <c r="H20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -1152,13 +1089,10 @@
       <c r="G21">
         <v>0</v>
       </c>
-      <c r="H21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -1178,13 +1112,10 @@
       <c r="G22">
         <v>1.02</v>
       </c>
-      <c r="H22">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B23">
         <v>2.38</v>
@@ -1204,13 +1135,10 @@
       <c r="G23">
         <v>1.6</v>
       </c>
-      <c r="H23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -1230,13 +1158,10 @@
       <c r="G24">
         <v>1.56</v>
       </c>
-      <c r="H24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B25">
         <v>4.86</v>
@@ -1256,13 +1181,10 @@
       <c r="G25">
         <v>2.05</v>
       </c>
-      <c r="H25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -1282,13 +1204,10 @@
       <c r="G26">
         <v>1.21</v>
       </c>
-      <c r="H26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
+    </row>
+    <row r="27" spans="1:7">
       <c r="A27" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -1308,13 +1227,10 @@
       <c r="G27">
         <v>1.7</v>
       </c>
-      <c r="H27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B28">
         <v>4.46</v>
@@ -1334,13 +1250,10 @@
       <c r="G28">
         <v>1.42</v>
       </c>
-      <c r="H28">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -1360,13 +1273,10 @@
       <c r="G29">
         <v>1.52</v>
       </c>
-      <c r="H29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8">
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B30">
         <v>1.79</v>
@@ -1386,13 +1296,10 @@
       <c r="G30">
         <v>1.01</v>
       </c>
-      <c r="H30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8">
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B31">
         <v>2.22</v>
@@ -1412,13 +1319,10 @@
       <c r="G31">
         <v>2.04</v>
       </c>
-      <c r="H31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
+    </row>
+    <row r="32" spans="1:7">
       <c r="A32" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B32">
         <v>0</v>
@@ -1438,13 +1342,10 @@
       <c r="G32">
         <v>1.65</v>
       </c>
-      <c r="H32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B33">
         <v>1.18</v>
@@ -1464,13 +1365,10 @@
       <c r="G33">
         <v>1.68</v>
       </c>
-      <c r="H33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
+    </row>
+    <row r="34" spans="1:7">
       <c r="A34" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -1490,13 +1388,10 @@
       <c r="G34">
         <v>0.89</v>
       </c>
-      <c r="H34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8">
+    </row>
+    <row r="35" spans="1:7">
       <c r="A35" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B35">
         <v>0</v>
@@ -1516,13 +1411,10 @@
       <c r="G35">
         <v>1.1</v>
       </c>
-      <c r="H35">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8">
+    </row>
+    <row r="36" spans="1:7">
       <c r="A36" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B36">
         <v>0</v>
@@ -1542,13 +1434,10 @@
       <c r="G36">
         <v>1.6</v>
       </c>
-      <c r="H36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8">
+    </row>
+    <row r="37" spans="1:7">
       <c r="A37" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B37">
         <v>4.49</v>
@@ -1568,13 +1457,10 @@
       <c r="G37">
         <v>1.44</v>
       </c>
-      <c r="H37">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8">
+    </row>
+    <row r="38" spans="1:7">
       <c r="A38" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -1594,13 +1480,10 @@
       <c r="G38">
         <v>1.74</v>
       </c>
-      <c r="H38">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8">
+    </row>
+    <row r="39" spans="1:7">
       <c r="A39" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B39">
         <v>4.76</v>
@@ -1620,13 +1503,10 @@
       <c r="G39">
         <v>1.73</v>
       </c>
-      <c r="H39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8">
+    </row>
+    <row r="40" spans="1:7">
       <c r="A40" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B40">
         <v>5.5</v>
@@ -1646,13 +1526,10 @@
       <c r="G40">
         <v>1.08</v>
       </c>
-      <c r="H40">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8">
+    </row>
+    <row r="41" spans="1:7">
       <c r="A41" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -1672,13 +1549,10 @@
       <c r="G41">
         <v>1.57</v>
       </c>
-      <c r="H41">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8">
+    </row>
+    <row r="42" spans="1:7">
       <c r="A42" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B42">
         <v>20.97</v>
@@ -1698,13 +1572,10 @@
       <c r="G42">
         <v>1.44</v>
       </c>
-      <c r="H42">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8">
+    </row>
+    <row r="43" spans="1:7">
       <c r="A43" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -1724,13 +1595,10 @@
       <c r="G43">
         <v>1.97</v>
       </c>
-      <c r="H43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8">
+    </row>
+    <row r="44" spans="1:7">
       <c r="A44" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -1750,13 +1618,10 @@
       <c r="G44">
         <v>1.78</v>
       </c>
-      <c r="H44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8">
+    </row>
+    <row r="45" spans="1:7">
       <c r="A45" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -1776,13 +1641,10 @@
       <c r="G45">
         <v>1.67</v>
       </c>
-      <c r="H45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8">
+    </row>
+    <row r="46" spans="1:7">
       <c r="A46" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B46">
         <v>0</v>
@@ -1802,13 +1664,10 @@
       <c r="G46">
         <v>1.19</v>
       </c>
-      <c r="H46">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8">
+    </row>
+    <row r="47" spans="1:7">
       <c r="A47" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -1828,13 +1687,10 @@
       <c r="G47">
         <v>0.95</v>
       </c>
-      <c r="H47">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8">
+    </row>
+    <row r="48" spans="1:7">
       <c r="A48" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -1854,13 +1710,10 @@
       <c r="G48">
         <v>1.91</v>
       </c>
-      <c r="H48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8">
+    </row>
+    <row r="49" spans="1:7">
       <c r="A49" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -1880,13 +1733,10 @@
       <c r="G49">
         <v>1.61</v>
       </c>
-      <c r="H49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8">
+    </row>
+    <row r="50" spans="1:7">
       <c r="A50" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B50">
         <v>5.25</v>
@@ -1906,13 +1756,10 @@
       <c r="G50">
         <v>1.54</v>
       </c>
-      <c r="H50">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8">
+    </row>
+    <row r="51" spans="1:7">
       <c r="A51" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B51">
         <v>0</v>
@@ -1932,13 +1779,10 @@
       <c r="G51">
         <v>1.76</v>
       </c>
-      <c r="H51">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8">
+    </row>
+    <row r="52" spans="1:7">
       <c r="A52" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B52">
         <v>0</v>
@@ -1958,13 +1802,10 @@
       <c r="G52">
         <v>1.28</v>
       </c>
-      <c r="H52">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8">
+    </row>
+    <row r="53" spans="1:7">
       <c r="A53" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B53">
         <v>7.22</v>
@@ -1984,13 +1825,10 @@
       <c r="G53">
         <v>1.53</v>
       </c>
-      <c r="H53">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8">
+    </row>
+    <row r="54" spans="1:7">
       <c r="A54" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B54">
         <v>0</v>
@@ -2010,13 +1848,10 @@
       <c r="G54">
         <v>1.56</v>
       </c>
-      <c r="H54">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8">
+    </row>
+    <row r="55" spans="1:7">
       <c r="A55" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B55">
         <v>3.89</v>
@@ -2036,13 +1871,10 @@
       <c r="G55">
         <v>2.07</v>
       </c>
-      <c r="H55">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8">
+    </row>
+    <row r="56" spans="1:7">
       <c r="A56" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B56">
         <v>0</v>
@@ -2062,13 +1894,10 @@
       <c r="G56">
         <v>1.9</v>
       </c>
-      <c r="H56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8">
+    </row>
+    <row r="57" spans="1:7">
       <c r="A57" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B57">
         <v>0</v>
@@ -2088,13 +1917,10 @@
       <c r="G57">
         <v>0.92</v>
       </c>
-      <c r="H57">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8">
+    </row>
+    <row r="58" spans="1:7">
       <c r="A58" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B58">
         <v>0</v>
@@ -2114,13 +1940,10 @@
       <c r="G58">
         <v>1.55</v>
       </c>
-      <c r="H58">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8">
+    </row>
+    <row r="59" spans="1:7">
       <c r="A59" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B59">
         <v>3.18</v>
@@ -2140,13 +1963,10 @@
       <c r="G59">
         <v>1.88</v>
       </c>
-      <c r="H59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8">
+    </row>
+    <row r="60" spans="1:7">
       <c r="A60" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B60">
         <v>0</v>
@@ -2166,13 +1986,10 @@
       <c r="G60">
         <v>0.78</v>
       </c>
-      <c r="H60">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8">
+    </row>
+    <row r="61" spans="1:7">
       <c r="A61" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B61">
         <v>6.81</v>
@@ -2192,13 +2009,10 @@
       <c r="G61">
         <v>1.29</v>
       </c>
-      <c r="H61">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8">
+    </row>
+    <row r="62" spans="1:7">
       <c r="A62" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B62">
         <v>8.06</v>
@@ -2218,13 +2032,10 @@
       <c r="G62">
         <v>1.73</v>
       </c>
-      <c r="H62">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8">
+    </row>
+    <row r="63" spans="1:7">
       <c r="A63" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B63">
         <v>2.08</v>
@@ -2243,9 +2054,6 @@
       </c>
       <c r="G63">
         <v>1.47</v>
-      </c>
-      <c r="H63">
-        <v>0.97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added uncertain DBSCAN clustering method to main_harmonic, main_katz and main_subgraph modules
</commit_message>
<xml_diff>
--- a/results/aucs/degree_centrality/aucs_degree_centrality_results.xlsx
+++ b/results/aucs/degree_centrality/aucs_degree_centrality_results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
   <si>
     <t>coauthor</t>
   </si>
@@ -29,6 +29,9 @@
   </si>
   <si>
     <t>work</t>
+  </si>
+  <si>
+    <t>cluster_class</t>
   </si>
   <si>
     <t>shannon_entropy</t>
@@ -604,13 +607,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G63"/>
+  <dimension ref="A1:H63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -629,10 +632,13 @@
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2">
         <v>1.43</v>
@@ -650,12 +656,15 @@
         <v>46.67</v>
       </c>
       <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
         <v>1.89</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3">
         <v>1.54</v>
@@ -673,12 +682,15 @@
         <v>36.15</v>
       </c>
       <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
         <v>1.95</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -696,12 +708,15 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>-1</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5">
         <v>1.79</v>
@@ -719,12 +734,15 @@
         <v>11.31</v>
       </c>
       <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
         <v>1.69</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -742,12 +760,15 @@
         <v>38.24</v>
       </c>
       <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
         <v>1.82</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -765,12 +786,15 @@
         <v>13.62</v>
       </c>
       <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
         <v>1.69</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B8">
         <v>9.82</v>
@@ -788,12 +812,15 @@
         <v>37.02</v>
       </c>
       <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
         <v>2.16</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -811,12 +838,15 @@
         <v>18.03</v>
       </c>
       <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
         <v>1.5</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -834,12 +864,15 @@
         <v>13.04</v>
       </c>
       <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
         <v>1.85</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B11">
         <v>3.62</v>
@@ -857,12 +890,15 @@
         <v>59.28</v>
       </c>
       <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
         <v>1.32</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -880,12 +916,15 @@
         <v>73.05</v>
       </c>
       <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
         <v>1.07</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -903,12 +942,15 @@
         <v>19.7</v>
       </c>
       <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
         <v>1.6</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -926,12 +968,15 @@
         <v>9.449999999999999</v>
       </c>
       <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
         <v>1.23</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B15">
         <v>6.87</v>
@@ -949,12 +994,15 @@
         <v>42.75</v>
       </c>
       <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
         <v>1.72</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B16">
         <v>7.87</v>
@@ -972,12 +1020,15 @@
         <v>46.98</v>
       </c>
       <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
         <v>1.74</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:8">
       <c r="A17" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B17">
         <v>1.65</v>
@@ -995,12 +1046,15 @@
         <v>9.09</v>
       </c>
       <c r="G17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
+        <v>-1</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B18">
         <v>5.25</v>
@@ -1018,12 +1072,15 @@
         <v>36.42</v>
       </c>
       <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
         <v>1.79</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:8">
       <c r="A19" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -1041,12 +1098,15 @@
         <v>91.67</v>
       </c>
       <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
         <v>0.41</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:8">
       <c r="A20" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -1064,12 +1124,15 @@
         <v>49.06</v>
       </c>
       <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20">
         <v>1.43</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:8">
       <c r="A21" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -1087,12 +1150,15 @@
         <v>100</v>
       </c>
       <c r="G21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
+        <v>-1</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -1110,12 +1176,15 @@
         <v>18.48</v>
       </c>
       <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
         <v>1.02</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:8">
       <c r="A23" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B23">
         <v>2.38</v>
@@ -1133,12 +1202,15 @@
         <v>8.33</v>
       </c>
       <c r="G23">
+        <v>-1</v>
+      </c>
+      <c r="H23">
         <v>1.6</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:8">
       <c r="A24" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -1156,12 +1228,15 @@
         <v>42.86</v>
       </c>
       <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24">
         <v>1.56</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:8">
       <c r="A25" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B25">
         <v>4.86</v>
@@ -1179,12 +1254,15 @@
         <v>13.89</v>
       </c>
       <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
         <v>2.05</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:8">
       <c r="A26" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -1202,12 +1280,15 @@
         <v>67.05</v>
       </c>
       <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="H26">
         <v>1.21</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:8">
       <c r="A27" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -1225,12 +1306,15 @@
         <v>16.78</v>
       </c>
       <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
         <v>1.7</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:8">
       <c r="A28" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B28">
         <v>4.46</v>
@@ -1248,12 +1332,15 @@
         <v>38.06</v>
       </c>
       <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="H28">
         <v>1.42</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:8">
       <c r="A29" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -1271,12 +1358,15 @@
         <v>48.28</v>
       </c>
       <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="H29">
         <v>1.52</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:8">
       <c r="A30" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B30">
         <v>1.79</v>
@@ -1294,12 +1384,15 @@
         <v>76.16</v>
       </c>
       <c r="G30">
+        <v>1</v>
+      </c>
+      <c r="H30">
         <v>1.01</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:8">
       <c r="A31" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B31">
         <v>2.22</v>
@@ -1317,12 +1410,15 @@
         <v>22.59</v>
       </c>
       <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
         <v>2.04</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:8">
       <c r="A32" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B32">
         <v>0</v>
@@ -1340,12 +1436,15 @@
         <v>12.21</v>
       </c>
       <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
         <v>1.65</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:8">
       <c r="A33" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B33">
         <v>1.18</v>
@@ -1363,12 +1462,15 @@
         <v>35.98</v>
       </c>
       <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
         <v>1.68</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:8">
       <c r="A34" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -1386,12 +1488,15 @@
         <v>69.09</v>
       </c>
       <c r="G34">
+        <v>1</v>
+      </c>
+      <c r="H34">
         <v>0.89</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:8">
       <c r="A35" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B35">
         <v>0</v>
@@ -1409,12 +1514,15 @@
         <v>5.39</v>
       </c>
       <c r="G35">
+        <v>-1</v>
+      </c>
+      <c r="H35">
         <v>1.1</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:8">
       <c r="A36" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B36">
         <v>0</v>
@@ -1432,12 +1540,15 @@
         <v>44.73</v>
       </c>
       <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36">
         <v>1.6</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:8">
       <c r="A37" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B37">
         <v>4.49</v>
@@ -1455,12 +1566,15 @@
         <v>20.97</v>
       </c>
       <c r="G37">
+        <v>1</v>
+      </c>
+      <c r="H37">
         <v>1.44</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:8">
       <c r="A38" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -1478,12 +1592,15 @@
         <v>16.21</v>
       </c>
       <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="H38">
         <v>1.74</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:8">
       <c r="A39" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B39">
         <v>4.76</v>
@@ -1501,12 +1618,15 @@
         <v>15.48</v>
       </c>
       <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="H39">
         <v>1.73</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:8">
       <c r="A40" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B40">
         <v>5.5</v>
@@ -1524,12 +1644,15 @@
         <v>24</v>
       </c>
       <c r="G40">
+        <v>1</v>
+      </c>
+      <c r="H40">
         <v>1.08</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:8">
       <c r="A41" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -1547,12 +1670,15 @@
         <v>24.77</v>
       </c>
       <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
         <v>1.57</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:8">
       <c r="A42" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B42">
         <v>20.97</v>
@@ -1570,12 +1696,15 @@
         <v>10.86</v>
       </c>
       <c r="G42">
+        <v>1</v>
+      </c>
+      <c r="H42">
         <v>1.44</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:8">
       <c r="A43" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -1593,12 +1722,15 @@
         <v>28.6</v>
       </c>
       <c r="G43">
+        <v>0</v>
+      </c>
+      <c r="H43">
         <v>1.97</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:8">
       <c r="A44" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -1616,12 +1748,15 @@
         <v>8.49</v>
       </c>
       <c r="G44">
+        <v>0</v>
+      </c>
+      <c r="H44">
         <v>1.78</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:8">
       <c r="A45" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -1639,12 +1774,15 @@
         <v>16.77</v>
       </c>
       <c r="G45">
+        <v>0</v>
+      </c>
+      <c r="H45">
         <v>1.67</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:8">
       <c r="A46" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B46">
         <v>0</v>
@@ -1662,12 +1800,15 @@
         <v>37.97</v>
       </c>
       <c r="G46">
+        <v>1</v>
+      </c>
+      <c r="H46">
         <v>1.19</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:8">
       <c r="A47" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -1685,12 +1826,15 @@
         <v>37.04</v>
       </c>
       <c r="G47">
+        <v>1</v>
+      </c>
+      <c r="H47">
         <v>0.95</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:8">
       <c r="A48" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -1708,12 +1852,15 @@
         <v>11.52</v>
       </c>
       <c r="G48">
+        <v>0</v>
+      </c>
+      <c r="H48">
         <v>1.91</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:8">
       <c r="A49" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -1731,12 +1878,15 @@
         <v>48.83</v>
       </c>
       <c r="G49">
+        <v>0</v>
+      </c>
+      <c r="H49">
         <v>1.61</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:8">
       <c r="A50" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B50">
         <v>5.25</v>
@@ -1754,12 +1904,15 @@
         <v>27.16</v>
       </c>
       <c r="G50">
+        <v>1</v>
+      </c>
+      <c r="H50">
         <v>1.54</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:8">
       <c r="A51" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B51">
         <v>0</v>
@@ -1777,12 +1930,15 @@
         <v>16.58</v>
       </c>
       <c r="G51">
+        <v>0</v>
+      </c>
+      <c r="H51">
         <v>1.76</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:8">
       <c r="A52" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B52">
         <v>0</v>
@@ -1800,12 +1956,15 @@
         <v>63.33</v>
       </c>
       <c r="G52">
+        <v>0</v>
+      </c>
+      <c r="H52">
         <v>1.28</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:8">
       <c r="A53" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B53">
         <v>7.22</v>
@@ -1823,12 +1982,15 @@
         <v>15.37</v>
       </c>
       <c r="G53">
+        <v>1</v>
+      </c>
+      <c r="H53">
         <v>1.53</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:8">
       <c r="A54" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B54">
         <v>0</v>
@@ -1846,12 +2008,15 @@
         <v>32.5</v>
       </c>
       <c r="G54">
+        <v>1</v>
+      </c>
+      <c r="H54">
         <v>1.56</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:8">
       <c r="A55" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B55">
         <v>3.89</v>
@@ -1869,12 +2034,15 @@
         <v>14.44</v>
       </c>
       <c r="G55">
+        <v>0</v>
+      </c>
+      <c r="H55">
         <v>2.07</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:8">
       <c r="A56" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B56">
         <v>0</v>
@@ -1892,12 +2060,15 @@
         <v>19.72</v>
       </c>
       <c r="G56">
+        <v>0</v>
+      </c>
+      <c r="H56">
         <v>1.9</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:8">
       <c r="A57" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B57">
         <v>0</v>
@@ -1915,12 +2086,15 @@
         <v>66.67</v>
       </c>
       <c r="G57">
+        <v>1</v>
+      </c>
+      <c r="H57">
         <v>0.92</v>
       </c>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:8">
       <c r="A58" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B58">
         <v>0</v>
@@ -1938,12 +2112,15 @@
         <v>27.44</v>
       </c>
       <c r="G58">
+        <v>1</v>
+      </c>
+      <c r="H58">
         <v>1.55</v>
       </c>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:8">
       <c r="A59" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B59">
         <v>3.18</v>
@@ -1961,12 +2138,15 @@
         <v>10.76</v>
       </c>
       <c r="G59">
+        <v>-1</v>
+      </c>
+      <c r="H59">
         <v>1.88</v>
       </c>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:8">
       <c r="A60" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B60">
         <v>0</v>
@@ -1984,12 +2164,15 @@
         <v>23.08</v>
       </c>
       <c r="G60">
+        <v>1</v>
+      </c>
+      <c r="H60">
         <v>0.78</v>
       </c>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:8">
       <c r="A61" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B61">
         <v>6.81</v>
@@ -2007,12 +2190,15 @@
         <v>46.6</v>
       </c>
       <c r="G61">
+        <v>1</v>
+      </c>
+      <c r="H61">
         <v>1.29</v>
       </c>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:8">
       <c r="A62" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B62">
         <v>8.06</v>
@@ -2030,12 +2216,15 @@
         <v>37</v>
       </c>
       <c r="G62">
+        <v>1</v>
+      </c>
+      <c r="H62">
         <v>1.73</v>
       </c>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:8">
       <c r="A63" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B63">
         <v>2.08</v>
@@ -2053,6 +2242,9 @@
         <v>32.35</v>
       </c>
       <c r="G63">
+        <v>0.33</v>
+      </c>
+      <c r="H63">
         <v>1.47</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added LayerCentralityExcelModel and refactored get_layer_centrality_excel_models method
</commit_message>
<xml_diff>
--- a/results/aucs/degree_centrality/aucs_degree_centrality_results.xlsx
+++ b/results/aucs/degree_centrality/aucs_degree_centrality_results.xlsx
@@ -7,14 +7,17 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="LayerCentrality" sheetId="1" r:id="rId1"/>
+    <sheet name="Layer Centrality" sheetId="1" r:id="rId1"/>
+    <sheet name="cluster_0" sheetId="2" r:id="rId2"/>
+    <sheet name="cluster_1" sheetId="3" r:id="rId3"/>
+    <sheet name="cluster_-1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="69">
   <si>
     <t>coauthor</t>
   </si>
@@ -31,10 +34,10 @@
     <t>work</t>
   </si>
   <si>
+    <t>shannon_entropy</t>
+  </si>
+  <si>
     <t>cluster_class</t>
-  </si>
-  <si>
-    <t>shannon_entropy</t>
   </si>
   <si>
     <t>U1</t>
@@ -656,10 +659,10 @@
         <v>46.67</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>1.89</v>
       </c>
       <c r="H2">
-        <v>1.89</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -682,10 +685,10 @@
         <v>36.15</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>1.95</v>
       </c>
       <c r="H3">
-        <v>1.95</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -708,10 +711,10 @@
         <v>0</v>
       </c>
       <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
         <v>-1</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -734,10 +737,10 @@
         <v>11.31</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>1.69</v>
       </c>
       <c r="H5">
-        <v>1.69</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -760,10 +763,10 @@
         <v>38.24</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>1.82</v>
       </c>
       <c r="H6">
-        <v>1.82</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -786,10 +789,10 @@
         <v>13.62</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>1.69</v>
       </c>
       <c r="H7">
-        <v>1.69</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -812,10 +815,10 @@
         <v>37.02</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>2.16</v>
       </c>
       <c r="H8">
-        <v>2.16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -838,10 +841,10 @@
         <v>18.03</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="H9">
-        <v>1.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -864,10 +867,10 @@
         <v>13.04</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>1.85</v>
       </c>
       <c r="H10">
-        <v>1.85</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -890,10 +893,10 @@
         <v>59.28</v>
       </c>
       <c r="G11">
-        <v>1</v>
+        <v>1.32</v>
       </c>
       <c r="H11">
-        <v>1.32</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -916,10 +919,10 @@
         <v>73.05</v>
       </c>
       <c r="G12">
-        <v>0</v>
+        <v>1.07</v>
       </c>
       <c r="H12">
-        <v>1.07</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -942,10 +945,10 @@
         <v>19.7</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>1.6</v>
       </c>
       <c r="H13">
-        <v>1.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -968,10 +971,10 @@
         <v>9.449999999999999</v>
       </c>
       <c r="G14">
-        <v>1</v>
+        <v>1.23</v>
       </c>
       <c r="H14">
-        <v>1.23</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -994,10 +997,10 @@
         <v>42.75</v>
       </c>
       <c r="G15">
-        <v>1</v>
+        <v>1.72</v>
       </c>
       <c r="H15">
-        <v>1.72</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -1020,10 +1023,10 @@
         <v>46.98</v>
       </c>
       <c r="G16">
-        <v>0</v>
+        <v>1.74</v>
       </c>
       <c r="H16">
-        <v>1.74</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -1046,10 +1049,10 @@
         <v>9.09</v>
       </c>
       <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
         <v>-1</v>
-      </c>
-      <c r="H17">
-        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -1072,10 +1075,10 @@
         <v>36.42</v>
       </c>
       <c r="G18">
-        <v>1</v>
+        <v>1.79</v>
       </c>
       <c r="H18">
-        <v>1.79</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -1098,10 +1101,10 @@
         <v>91.67</v>
       </c>
       <c r="G19">
-        <v>1</v>
+        <v>0.41</v>
       </c>
       <c r="H19">
-        <v>0.41</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -1124,10 +1127,10 @@
         <v>49.06</v>
       </c>
       <c r="G20">
-        <v>1</v>
+        <v>1.43</v>
       </c>
       <c r="H20">
-        <v>1.43</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -1150,10 +1153,10 @@
         <v>100</v>
       </c>
       <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
         <v>-1</v>
-      </c>
-      <c r="H21">
-        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -1176,10 +1179,10 @@
         <v>18.48</v>
       </c>
       <c r="G22">
-        <v>1</v>
+        <v>1.02</v>
       </c>
       <c r="H22">
-        <v>1.02</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -1202,10 +1205,10 @@
         <v>8.33</v>
       </c>
       <c r="G23">
+        <v>1.6</v>
+      </c>
+      <c r="H23">
         <v>-1</v>
-      </c>
-      <c r="H23">
-        <v>1.6</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1228,10 +1231,10 @@
         <v>42.86</v>
       </c>
       <c r="G24">
-        <v>1</v>
+        <v>1.56</v>
       </c>
       <c r="H24">
-        <v>1.56</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1254,10 +1257,10 @@
         <v>13.89</v>
       </c>
       <c r="G25">
-        <v>0</v>
+        <v>2.05</v>
       </c>
       <c r="H25">
-        <v>2.05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1280,10 +1283,10 @@
         <v>67.05</v>
       </c>
       <c r="G26">
-        <v>1</v>
+        <v>1.21</v>
       </c>
       <c r="H26">
-        <v>1.21</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -1306,10 +1309,10 @@
         <v>16.78</v>
       </c>
       <c r="G27">
-        <v>0</v>
+        <v>1.7</v>
       </c>
       <c r="H27">
-        <v>1.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1332,10 +1335,10 @@
         <v>38.06</v>
       </c>
       <c r="G28">
-        <v>1</v>
+        <v>1.42</v>
       </c>
       <c r="H28">
-        <v>1.42</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -1358,10 +1361,10 @@
         <v>48.28</v>
       </c>
       <c r="G29">
-        <v>1</v>
+        <v>1.52</v>
       </c>
       <c r="H29">
-        <v>1.52</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1384,10 +1387,10 @@
         <v>76.16</v>
       </c>
       <c r="G30">
-        <v>1</v>
+        <v>1.01</v>
       </c>
       <c r="H30">
-        <v>1.01</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1410,10 +1413,10 @@
         <v>22.59</v>
       </c>
       <c r="G31">
-        <v>0</v>
+        <v>2.04</v>
       </c>
       <c r="H31">
-        <v>2.04</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1436,10 +1439,10 @@
         <v>12.21</v>
       </c>
       <c r="G32">
-        <v>0</v>
+        <v>1.65</v>
       </c>
       <c r="H32">
-        <v>1.65</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -1462,10 +1465,10 @@
         <v>35.98</v>
       </c>
       <c r="G33">
-        <v>0</v>
+        <v>1.68</v>
       </c>
       <c r="H33">
-        <v>1.68</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -1488,10 +1491,10 @@
         <v>69.09</v>
       </c>
       <c r="G34">
-        <v>1</v>
+        <v>0.89</v>
       </c>
       <c r="H34">
-        <v>0.89</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -1514,10 +1517,10 @@
         <v>5.39</v>
       </c>
       <c r="G35">
+        <v>1.1</v>
+      </c>
+      <c r="H35">
         <v>-1</v>
-      </c>
-      <c r="H35">
-        <v>1.1</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -1540,10 +1543,10 @@
         <v>44.73</v>
       </c>
       <c r="G36">
-        <v>0</v>
+        <v>1.6</v>
       </c>
       <c r="H36">
-        <v>1.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -1566,10 +1569,10 @@
         <v>20.97</v>
       </c>
       <c r="G37">
-        <v>1</v>
+        <v>1.44</v>
       </c>
       <c r="H37">
-        <v>1.44</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -1592,10 +1595,10 @@
         <v>16.21</v>
       </c>
       <c r="G38">
-        <v>0</v>
+        <v>1.74</v>
       </c>
       <c r="H38">
-        <v>1.74</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -1618,10 +1621,10 @@
         <v>15.48</v>
       </c>
       <c r="G39">
-        <v>0</v>
+        <v>1.73</v>
       </c>
       <c r="H39">
-        <v>1.73</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -1644,10 +1647,10 @@
         <v>24</v>
       </c>
       <c r="G40">
-        <v>1</v>
+        <v>1.08</v>
       </c>
       <c r="H40">
-        <v>1.08</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -1670,10 +1673,10 @@
         <v>24.77</v>
       </c>
       <c r="G41">
-        <v>0</v>
+        <v>1.57</v>
       </c>
       <c r="H41">
-        <v>1.57</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -1696,10 +1699,10 @@
         <v>10.86</v>
       </c>
       <c r="G42">
-        <v>1</v>
+        <v>1.44</v>
       </c>
       <c r="H42">
-        <v>1.44</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -1722,10 +1725,10 @@
         <v>28.6</v>
       </c>
       <c r="G43">
-        <v>0</v>
+        <v>1.97</v>
       </c>
       <c r="H43">
-        <v>1.97</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -1748,10 +1751,10 @@
         <v>8.49</v>
       </c>
       <c r="G44">
-        <v>0</v>
+        <v>1.78</v>
       </c>
       <c r="H44">
-        <v>1.78</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -1774,10 +1777,10 @@
         <v>16.77</v>
       </c>
       <c r="G45">
-        <v>0</v>
+        <v>1.67</v>
       </c>
       <c r="H45">
-        <v>1.67</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -1800,10 +1803,10 @@
         <v>37.97</v>
       </c>
       <c r="G46">
-        <v>1</v>
+        <v>1.19</v>
       </c>
       <c r="H46">
-        <v>1.19</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -1826,10 +1829,10 @@
         <v>37.04</v>
       </c>
       <c r="G47">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="H47">
-        <v>0.95</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -1852,10 +1855,10 @@
         <v>11.52</v>
       </c>
       <c r="G48">
-        <v>0</v>
+        <v>1.91</v>
       </c>
       <c r="H48">
-        <v>1.91</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -1878,10 +1881,10 @@
         <v>48.83</v>
       </c>
       <c r="G49">
-        <v>0</v>
+        <v>1.61</v>
       </c>
       <c r="H49">
-        <v>1.61</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -1904,10 +1907,10 @@
         <v>27.16</v>
       </c>
       <c r="G50">
-        <v>1</v>
+        <v>1.54</v>
       </c>
       <c r="H50">
-        <v>1.54</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -1930,10 +1933,10 @@
         <v>16.58</v>
       </c>
       <c r="G51">
-        <v>0</v>
+        <v>1.76</v>
       </c>
       <c r="H51">
-        <v>1.76</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -1956,10 +1959,10 @@
         <v>63.33</v>
       </c>
       <c r="G52">
-        <v>0</v>
+        <v>1.28</v>
       </c>
       <c r="H52">
-        <v>1.28</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:8">
@@ -1982,10 +1985,10 @@
         <v>15.37</v>
       </c>
       <c r="G53">
-        <v>1</v>
+        <v>1.53</v>
       </c>
       <c r="H53">
-        <v>1.53</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:8">
@@ -2008,10 +2011,10 @@
         <v>32.5</v>
       </c>
       <c r="G54">
-        <v>1</v>
+        <v>1.56</v>
       </c>
       <c r="H54">
-        <v>1.56</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:8">
@@ -2034,10 +2037,10 @@
         <v>14.44</v>
       </c>
       <c r="G55">
-        <v>0</v>
+        <v>2.07</v>
       </c>
       <c r="H55">
-        <v>2.07</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:8">
@@ -2060,10 +2063,10 @@
         <v>19.72</v>
       </c>
       <c r="G56">
-        <v>0</v>
+        <v>1.9</v>
       </c>
       <c r="H56">
-        <v>1.9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:8">
@@ -2086,10 +2089,10 @@
         <v>66.67</v>
       </c>
       <c r="G57">
-        <v>1</v>
+        <v>0.92</v>
       </c>
       <c r="H57">
-        <v>0.92</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:8">
@@ -2112,10 +2115,10 @@
         <v>27.44</v>
       </c>
       <c r="G58">
-        <v>1</v>
+        <v>1.55</v>
       </c>
       <c r="H58">
-        <v>1.55</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:8">
@@ -2138,10 +2141,10 @@
         <v>10.76</v>
       </c>
       <c r="G59">
+        <v>1.88</v>
+      </c>
+      <c r="H59">
         <v>-1</v>
-      </c>
-      <c r="H59">
-        <v>1.88</v>
       </c>
     </row>
     <row r="60" spans="1:8">
@@ -2164,10 +2167,10 @@
         <v>23.08</v>
       </c>
       <c r="G60">
-        <v>1</v>
+        <v>0.78</v>
       </c>
       <c r="H60">
-        <v>0.78</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:8">
@@ -2190,10 +2193,10 @@
         <v>46.6</v>
       </c>
       <c r="G61">
-        <v>1</v>
+        <v>1.29</v>
       </c>
       <c r="H61">
-        <v>1.29</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:8">
@@ -2216,10 +2219,10 @@
         <v>37</v>
       </c>
       <c r="G62">
-        <v>1</v>
+        <v>1.73</v>
       </c>
       <c r="H62">
-        <v>1.73</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:8">
@@ -2242,10 +2245,10 @@
         <v>32.35</v>
       </c>
       <c r="G63">
+        <v>1.47</v>
+      </c>
+      <c r="H63">
         <v>0.33</v>
-      </c>
-      <c r="H63">
-        <v>1.47</v>
       </c>
     </row>
   </sheetData>
@@ -2265,4 +2268,1818 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>1.43</v>
+      </c>
+      <c r="C2">
+        <v>21.67</v>
+      </c>
+      <c r="D2">
+        <v>12.14</v>
+      </c>
+      <c r="E2">
+        <v>18.1</v>
+      </c>
+      <c r="F2">
+        <v>46.67</v>
+      </c>
+      <c r="G2">
+        <v>1.89</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>1.54</v>
+      </c>
+      <c r="C3">
+        <v>24.62</v>
+      </c>
+      <c r="D3">
+        <v>28.46</v>
+      </c>
+      <c r="E3">
+        <v>9.23</v>
+      </c>
+      <c r="F3">
+        <v>36.15</v>
+      </c>
+      <c r="G3">
+        <v>1.95</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>1.79</v>
+      </c>
+      <c r="C4">
+        <v>46.43</v>
+      </c>
+      <c r="D4">
+        <v>4.17</v>
+      </c>
+      <c r="E4">
+        <v>36.31</v>
+      </c>
+      <c r="F4">
+        <v>11.31</v>
+      </c>
+      <c r="G4">
+        <v>1.69</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>34.76</v>
+      </c>
+      <c r="D5">
+        <v>17.59</v>
+      </c>
+      <c r="E5">
+        <v>9.41</v>
+      </c>
+      <c r="F5">
+        <v>38.24</v>
+      </c>
+      <c r="G5">
+        <v>1.82</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>19.43</v>
+      </c>
+      <c r="D6">
+        <v>11.77</v>
+      </c>
+      <c r="E6">
+        <v>55.18</v>
+      </c>
+      <c r="F6">
+        <v>13.62</v>
+      </c>
+      <c r="G6">
+        <v>1.69</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7">
+        <v>9.82</v>
+      </c>
+      <c r="C7">
+        <v>23.86</v>
+      </c>
+      <c r="D7">
+        <v>14.21</v>
+      </c>
+      <c r="E7">
+        <v>15.09</v>
+      </c>
+      <c r="F7">
+        <v>37.02</v>
+      </c>
+      <c r="G7">
+        <v>2.16</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>42.62</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>39.34</v>
+      </c>
+      <c r="F8">
+        <v>18.03</v>
+      </c>
+      <c r="G8">
+        <v>1.5</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>38.72</v>
+      </c>
+      <c r="D9">
+        <v>15.11</v>
+      </c>
+      <c r="E9">
+        <v>33.13</v>
+      </c>
+      <c r="F9">
+        <v>13.04</v>
+      </c>
+      <c r="G9">
+        <v>1.85</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>19.6</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>7.35</v>
+      </c>
+      <c r="F10">
+        <v>73.05</v>
+      </c>
+      <c r="G10">
+        <v>1.07</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>58.81</v>
+      </c>
+      <c r="D11">
+        <v>10.75</v>
+      </c>
+      <c r="E11">
+        <v>10.75</v>
+      </c>
+      <c r="F11">
+        <v>19.7</v>
+      </c>
+      <c r="G11">
+        <v>1.6</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12">
+        <v>7.87</v>
+      </c>
+      <c r="C12">
+        <v>29.66</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>15.49</v>
+      </c>
+      <c r="F12">
+        <v>46.98</v>
+      </c>
+      <c r="G12">
+        <v>1.74</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13">
+        <v>4.86</v>
+      </c>
+      <c r="C13">
+        <v>34.03</v>
+      </c>
+      <c r="D13">
+        <v>13.19</v>
+      </c>
+      <c r="E13">
+        <v>34.03</v>
+      </c>
+      <c r="F13">
+        <v>13.89</v>
+      </c>
+      <c r="G13">
+        <v>2.05</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>29.02</v>
+      </c>
+      <c r="D14">
+        <v>6.12</v>
+      </c>
+      <c r="E14">
+        <v>48.07</v>
+      </c>
+      <c r="F14">
+        <v>16.78</v>
+      </c>
+      <c r="G14">
+        <v>1.7</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15">
+        <v>2.22</v>
+      </c>
+      <c r="C15">
+        <v>33.7</v>
+      </c>
+      <c r="D15">
+        <v>13.33</v>
+      </c>
+      <c r="E15">
+        <v>28.15</v>
+      </c>
+      <c r="F15">
+        <v>22.59</v>
+      </c>
+      <c r="G15">
+        <v>2.04</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>44.39</v>
+      </c>
+      <c r="D16">
+        <v>5.61</v>
+      </c>
+      <c r="E16">
+        <v>37.79</v>
+      </c>
+      <c r="F16">
+        <v>12.21</v>
+      </c>
+      <c r="G16">
+        <v>1.65</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17">
+        <v>1.18</v>
+      </c>
+      <c r="C17">
+        <v>44.8</v>
+      </c>
+      <c r="D17">
+        <v>2.65</v>
+      </c>
+      <c r="E17">
+        <v>15.39</v>
+      </c>
+      <c r="F17">
+        <v>35.98</v>
+      </c>
+      <c r="G17">
+        <v>1.68</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>29.65</v>
+      </c>
+      <c r="D18">
+        <v>0.85</v>
+      </c>
+      <c r="E18">
+        <v>24.77</v>
+      </c>
+      <c r="F18">
+        <v>44.73</v>
+      </c>
+      <c r="G18">
+        <v>1.6</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>16.21</v>
+      </c>
+      <c r="D19">
+        <v>14.36</v>
+      </c>
+      <c r="E19">
+        <v>53.22</v>
+      </c>
+      <c r="F19">
+        <v>16.21</v>
+      </c>
+      <c r="G19">
+        <v>1.74</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20">
+        <v>4.76</v>
+      </c>
+      <c r="C20">
+        <v>55.95</v>
+      </c>
+      <c r="D20">
+        <v>3.57</v>
+      </c>
+      <c r="E20">
+        <v>20.24</v>
+      </c>
+      <c r="F20">
+        <v>15.48</v>
+      </c>
+      <c r="G20">
+        <v>1.73</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>13.46</v>
+      </c>
+      <c r="D21">
+        <v>5.2</v>
+      </c>
+      <c r="E21">
+        <v>56.57</v>
+      </c>
+      <c r="F21">
+        <v>24.77</v>
+      </c>
+      <c r="G21">
+        <v>1.57</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>29.95</v>
+      </c>
+      <c r="D22">
+        <v>17.97</v>
+      </c>
+      <c r="E22">
+        <v>23.48</v>
+      </c>
+      <c r="F22">
+        <v>28.6</v>
+      </c>
+      <c r="G22">
+        <v>1.97</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>32.09</v>
+      </c>
+      <c r="D23">
+        <v>16.15</v>
+      </c>
+      <c r="E23">
+        <v>43.27</v>
+      </c>
+      <c r="F23">
+        <v>8.49</v>
+      </c>
+      <c r="G23">
+        <v>1.78</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>27.54</v>
+      </c>
+      <c r="D24">
+        <v>5.39</v>
+      </c>
+      <c r="E24">
+        <v>50.3</v>
+      </c>
+      <c r="F24">
+        <v>16.77</v>
+      </c>
+      <c r="G24">
+        <v>1.67</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>25.31</v>
+      </c>
+      <c r="D25">
+        <v>34.36</v>
+      </c>
+      <c r="E25">
+        <v>28.81</v>
+      </c>
+      <c r="F25">
+        <v>11.52</v>
+      </c>
+      <c r="G25">
+        <v>1.91</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>28.73</v>
+      </c>
+      <c r="D26">
+        <v>2.34</v>
+      </c>
+      <c r="E26">
+        <v>20.1</v>
+      </c>
+      <c r="F26">
+        <v>48.83</v>
+      </c>
+      <c r="G26">
+        <v>1.61</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>36.45</v>
+      </c>
+      <c r="D27">
+        <v>7.22</v>
+      </c>
+      <c r="E27">
+        <v>39.74</v>
+      </c>
+      <c r="F27">
+        <v>16.58</v>
+      </c>
+      <c r="G27">
+        <v>1.76</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>24.52</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>12.14</v>
+      </c>
+      <c r="F28">
+        <v>63.33</v>
+      </c>
+      <c r="G28">
+        <v>1.28</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B29">
+        <v>3.89</v>
+      </c>
+      <c r="C29">
+        <v>33.89</v>
+      </c>
+      <c r="D29">
+        <v>17.22</v>
+      </c>
+      <c r="E29">
+        <v>30.56</v>
+      </c>
+      <c r="F29">
+        <v>14.44</v>
+      </c>
+      <c r="G29">
+        <v>2.07</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>36.7</v>
+      </c>
+      <c r="D30">
+        <v>13.3</v>
+      </c>
+      <c r="E30">
+        <v>30.28</v>
+      </c>
+      <c r="F30">
+        <v>19.72</v>
+      </c>
+      <c r="G30">
+        <v>1.9</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B31">
+        <v>1.357241379310345</v>
+      </c>
+      <c r="C31">
+        <v>32.29551724137932</v>
+      </c>
+      <c r="D31">
+        <v>10.10448275862069</v>
+      </c>
+      <c r="E31">
+        <v>29.18241379310344</v>
+      </c>
+      <c r="F31">
+        <v>27.0596551724138</v>
+      </c>
+      <c r="G31">
+        <v>1.747241379310344</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2:F30">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThanOrEqual">
+      <formula>75</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThanOrEqual">
+      <formula>50</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThanOrEqual">
+      <formula>30</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThanOrEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2">
+        <v>3.62</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>3.62</v>
+      </c>
+      <c r="E2">
+        <v>33.48</v>
+      </c>
+      <c r="F2">
+        <v>59.28</v>
+      </c>
+      <c r="G2">
+        <v>1.32</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>25.87</v>
+      </c>
+      <c r="E3">
+        <v>64.68000000000001</v>
+      </c>
+      <c r="F3">
+        <v>9.449999999999999</v>
+      </c>
+      <c r="G3">
+        <v>1.23</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4">
+        <v>6.87</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>14.5</v>
+      </c>
+      <c r="E4">
+        <v>35.88</v>
+      </c>
+      <c r="F4">
+        <v>42.75</v>
+      </c>
+      <c r="G4">
+        <v>1.72</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5">
+        <v>5.25</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>27.16</v>
+      </c>
+      <c r="E5">
+        <v>31.17</v>
+      </c>
+      <c r="F5">
+        <v>36.42</v>
+      </c>
+      <c r="G5">
+        <v>1.79</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>8.33</v>
+      </c>
+      <c r="F6">
+        <v>91.67</v>
+      </c>
+      <c r="G6">
+        <v>0.41</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>14.15</v>
+      </c>
+      <c r="E7">
+        <v>36.79</v>
+      </c>
+      <c r="F7">
+        <v>49.06</v>
+      </c>
+      <c r="G7">
+        <v>1.43</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>6.52</v>
+      </c>
+      <c r="E8">
+        <v>75</v>
+      </c>
+      <c r="F8">
+        <v>18.48</v>
+      </c>
+      <c r="G8">
+        <v>1.02</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>29.76</v>
+      </c>
+      <c r="E9">
+        <v>27.38</v>
+      </c>
+      <c r="F9">
+        <v>42.86</v>
+      </c>
+      <c r="G9">
+        <v>1.56</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>10.23</v>
+      </c>
+      <c r="E10">
+        <v>22.73</v>
+      </c>
+      <c r="F10">
+        <v>67.05</v>
+      </c>
+      <c r="G10">
+        <v>1.21</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11">
+        <v>4.46</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>4.46</v>
+      </c>
+      <c r="E11">
+        <v>53.02</v>
+      </c>
+      <c r="F11">
+        <v>38.06</v>
+      </c>
+      <c r="G11">
+        <v>1.42</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>25.86</v>
+      </c>
+      <c r="E12">
+        <v>25.86</v>
+      </c>
+      <c r="F12">
+        <v>48.28</v>
+      </c>
+      <c r="G12">
+        <v>1.52</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13">
+        <v>1.79</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>2.85</v>
+      </c>
+      <c r="E13">
+        <v>19.2</v>
+      </c>
+      <c r="F13">
+        <v>76.16</v>
+      </c>
+      <c r="G13">
+        <v>1.01</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>30.91</v>
+      </c>
+      <c r="F14">
+        <v>69.09</v>
+      </c>
+      <c r="G14">
+        <v>0.89</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15">
+        <v>4.49</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>10.86</v>
+      </c>
+      <c r="E15">
+        <v>63.67</v>
+      </c>
+      <c r="F15">
+        <v>20.97</v>
+      </c>
+      <c r="G15">
+        <v>1.44</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16">
+        <v>5.5</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>70.5</v>
+      </c>
+      <c r="F16">
+        <v>24</v>
+      </c>
+      <c r="G16">
+        <v>1.08</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17">
+        <v>20.97</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>4.49</v>
+      </c>
+      <c r="E17">
+        <v>63.67</v>
+      </c>
+      <c r="F17">
+        <v>10.86</v>
+      </c>
+      <c r="G17">
+        <v>1.44</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>4.51</v>
+      </c>
+      <c r="E18">
+        <v>57.52</v>
+      </c>
+      <c r="F18">
+        <v>37.97</v>
+      </c>
+      <c r="G18">
+        <v>1.19</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>62.96</v>
+      </c>
+      <c r="F19">
+        <v>37.04</v>
+      </c>
+      <c r="G19">
+        <v>0.95</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20">
+        <v>5.25</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>10.49</v>
+      </c>
+      <c r="E20">
+        <v>57.1</v>
+      </c>
+      <c r="F20">
+        <v>27.16</v>
+      </c>
+      <c r="G20">
+        <v>1.54</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21">
+        <v>7.22</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>15.37</v>
+      </c>
+      <c r="E21">
+        <v>62.04</v>
+      </c>
+      <c r="F21">
+        <v>15.37</v>
+      </c>
+      <c r="G21">
+        <v>1.53</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>41.87</v>
+      </c>
+      <c r="E22">
+        <v>25.62</v>
+      </c>
+      <c r="F22">
+        <v>32.5</v>
+      </c>
+      <c r="G22">
+        <v>1.56</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>33.33</v>
+      </c>
+      <c r="F23">
+        <v>66.67</v>
+      </c>
+      <c r="G23">
+        <v>0.92</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>28.35</v>
+      </c>
+      <c r="E24">
+        <v>44.21</v>
+      </c>
+      <c r="F24">
+        <v>27.44</v>
+      </c>
+      <c r="G24">
+        <v>1.55</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>76.92</v>
+      </c>
+      <c r="F25">
+        <v>23.08</v>
+      </c>
+      <c r="G25">
+        <v>0.78</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26">
+        <v>6.81</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>46.6</v>
+      </c>
+      <c r="F26">
+        <v>46.6</v>
+      </c>
+      <c r="G26">
+        <v>1.29</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B27">
+        <v>8.06</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>13</v>
+      </c>
+      <c r="E27">
+        <v>41.94</v>
+      </c>
+      <c r="F27">
+        <v>37</v>
+      </c>
+      <c r="G27">
+        <v>1.73</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28">
+        <v>3.088076923076923</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>11.30461538461538</v>
+      </c>
+      <c r="E28">
+        <v>45.01961538461538</v>
+      </c>
+      <c r="F28">
+        <v>40.58730769230769</v>
+      </c>
+      <c r="G28">
+        <v>1.289615384615385</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2:F27">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThanOrEqual">
+      <formula>75</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThanOrEqual">
+      <formula>50</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThanOrEqual">
+      <formula>30</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThanOrEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>100</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3">
+        <v>1.65</v>
+      </c>
+      <c r="C3">
+        <v>9.5</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>79.75</v>
+      </c>
+      <c r="F3">
+        <v>9.09</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>100</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5">
+        <v>2.38</v>
+      </c>
+      <c r="C5">
+        <v>63.1</v>
+      </c>
+      <c r="D5">
+        <v>16.67</v>
+      </c>
+      <c r="E5">
+        <v>9.52</v>
+      </c>
+      <c r="F5">
+        <v>8.33</v>
+      </c>
+      <c r="G5">
+        <v>1.6</v>
+      </c>
+      <c r="H5">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>25.49</v>
+      </c>
+      <c r="E6">
+        <v>69.12</v>
+      </c>
+      <c r="F6">
+        <v>5.39</v>
+      </c>
+      <c r="G6">
+        <v>1.1</v>
+      </c>
+      <c r="H6">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7">
+        <v>3.18</v>
+      </c>
+      <c r="C7">
+        <v>42.58</v>
+      </c>
+      <c r="D7">
+        <v>34.24</v>
+      </c>
+      <c r="E7">
+        <v>9.24</v>
+      </c>
+      <c r="F7">
+        <v>10.76</v>
+      </c>
+      <c r="G7">
+        <v>1.88</v>
+      </c>
+      <c r="H7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8">
+        <v>1.201666666666666</v>
+      </c>
+      <c r="C8">
+        <v>19.19666666666667</v>
+      </c>
+      <c r="D8">
+        <v>12.73333333333333</v>
+      </c>
+      <c r="E8">
+        <v>44.605</v>
+      </c>
+      <c r="F8">
+        <v>22.26166666666667</v>
+      </c>
+      <c r="G8">
+        <v>0.93</v>
+      </c>
+      <c r="H8">
+        <v>-1</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2:F7">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThanOrEqual">
+      <formula>75</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThanOrEqual">
+      <formula>50</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThanOrEqual">
+      <formula>30</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThanOrEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>